<commit_message>
nhsrc checklists and sql files
</commit_message>
<xml_diff>
--- a/jss/cg/CG-NQAS-CHC-BSU-English.xlsx
+++ b/jss/cg/CG-NQAS-CHC-BSU-English.xlsx
@@ -245,7 +245,7 @@
     <t xml:space="preserve">PI/SI/RR</t>
   </si>
   <si>
-    <t xml:space="preserve">Area of Concern C: Inputs</t>
+    <t xml:space="preserve">Area of Concern C Inputs</t>
   </si>
   <si>
     <t xml:space="preserve">Standard C1.</t>
@@ -1607,6 +1607,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2126,7 +2127,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2249,21 +2250,21 @@
   </sheetPr>
   <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.5663265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6785714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="8.48469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="8.36224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>